<commit_message>
algo.java has method and linklist
</commit_message>
<xml_diff>
--- a/movieCatcher/js/algo.xlsx
+++ b/movieCatcher/js/algo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -586,14 +586,14 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
+      <c r="E3" s="7"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="6"/>
     </row>
@@ -629,8 +629,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7">
+      <c r="H5" s="7">
         <v>1</v>
       </c>
       <c r="J5" s="3"/>
@@ -648,8 +647,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="7">
+      <c r="I6" s="7">
         <v>1</v>
       </c>
       <c r="K6" s="4"/>

</xml_diff>

<commit_message>
algo.java can produce link by xiao
</commit_message>
<xml_diff>
--- a/movieCatcher/js/algo.xlsx
+++ b/movieCatcher/js/algo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,51 +16,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
-  <si>
-    <t>A-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B-2</t>
-  </si>
-  <si>
-    <t>B-3</t>
-  </si>
-  <si>
-    <t>C-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C-2</t>
-  </si>
-  <si>
-    <t>C-3</t>
-  </si>
-  <si>
-    <t>C-4</t>
-  </si>
-  <si>
-    <t>C-5</t>
-  </si>
-  <si>
-    <t>B-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie[0][0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>movie[9][8]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+  <si>
+    <t>0-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1-1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(1-2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-1(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-2(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-1(3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-2(4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-3(5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C-1(6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C-2(7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C-3(8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C-4(9)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C-5(10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-2(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1-4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>graph[10][9]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -514,63 +532,69 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="7.625" customWidth="1"/>
+    <col min="1" max="9" width="7.625" customWidth="1"/>
+    <col min="10" max="10" width="10.875" customWidth="1"/>
+    <col min="11" max="11" width="7.625" customWidth="1"/>
     <col min="12" max="12" width="1.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -581,7 +605,7 @@
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -599,7 +623,7 @@
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -619,7 +643,7 @@
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -638,7 +662,7 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -655,7 +679,7 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -673,7 +697,7 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -691,7 +715,7 @@
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -709,7 +733,7 @@
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -727,7 +751,7 @@
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -738,7 +762,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="2"/>

</xml_diff>